<commit_message>
Fix total price calculation in Excel template.
</commit_message>
<xml_diff>
--- a/templates/ecommerce/template.xlsx
+++ b/templates/ecommerce/template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <r>
       <rPr>
@@ -30,9 +30,9 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="204"/>
+        <charset val="1"/>
       </rPr>
-      <t>ПРАЙС-ЛИСТ </t>
+      <t xml:space="preserve">ПРАЙС-ЛИСТ </t>
     </r>
     <r>
       <rPr>
@@ -41,9 +41,9 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="204"/>
+        <charset val="1"/>
       </rPr>
-      <t> 
+      <t xml:space="preserve"> 
 ООО "Исток-Плюс" 
 (812) 416-32-00</t>
     </r>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t xml:space="preserve">Цены указаны на:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.08.2016</t>
   </si>
   <si>
     <t xml:space="preserve">Итого товара:</t>
@@ -103,7 +106,7 @@
     <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
     <numFmt numFmtId="166" formatCode="#,##0.00&quot; р.&quot;"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -132,7 +135,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -140,7 +143,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="16"/>
@@ -150,7 +160,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -159,12 +169,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDBEEF4"/>
+        <fgColor rgb="FFBABABA"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDAEEF3"/>
         <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -173,84 +189,14 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
+      <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="medium"/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -274,108 +220,88 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="6" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="2" borderId="7" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="8" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in 20% - Accent5" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -393,12 +319,12 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFBABABA"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFDBEEF4"/>
+      <rgbColor rgb="FFDAEEF3"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
@@ -448,177 +374,203 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.3481781376518"/>
     <col collapsed="false" hidden="true" max="2" min="2" style="0" width="0"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.2105263157895"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="10" min="8" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.497975708502"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="10" min="8" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="0"/>
-      <c r="I1" s="0"/>
-      <c r="J1" s="0"/>
-      <c r="K1" s="0"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="0"/>
-      <c r="I2" s="0"/>
-      <c r="J2" s="0"/>
-      <c r="K2" s="0"/>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="0"/>
-      <c r="I3" s="0"/>
-      <c r="J3" s="0"/>
-      <c r="K3" s="0"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="3" t="s">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="21.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+    <row r="5" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="6" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="7" t="n">
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="8" t="n">
         <f aca="false">SUM(G9:G100000)</f>
         <v>0</v>
       </c>
-      <c r="H5" s="0"/>
-      <c r="I5" s="0"/>
-      <c r="J5" s="0"/>
-      <c r="K5" s="0"/>
-    </row>
-    <row r="6" s="14" customFormat="true" ht="21.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H5" s="2" t="n">
+        <f aca="false">SUM(H9:H3448)</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <f aca="false">SUM(I9:I3448)</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <f aca="false">SUM(J9:J3448)</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="3" t="n">
+        <f aca="false">SUM(K9:K3448)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" s="15" customFormat="true" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="10" t="n">
-        <f aca="false">SUM(H9:I35)</f>
+        <f aca="false">MIN(H6:K6)</f>
         <v>0</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G6" s="12" t="str">
         <f aca="false">IF(E6&gt;K8,F8,IF(E6&gt;J8,E8,IF(E6&gt;I8,D8,C8)))</f>
         <v>розница</v>
       </c>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
+      <c r="H6" s="13" t="str">
+        <f aca="false">IF(H5&gt;H8,H5,J4)</f>
+        <v>NaN</v>
+      </c>
+      <c r="I6" s="13" t="str">
+        <f aca="false">IF(I5&gt;I8,I5,J4)</f>
+        <v>NaN</v>
+      </c>
+      <c r="J6" s="13" t="str">
+        <f aca="false">IF(J5&gt;J8,J5,J4)</f>
+        <v>NaN</v>
+      </c>
+      <c r="K6" s="14" t="str">
+        <f aca="false">IF(K5&gt;K8,K5,J4)</f>
+        <v>NaN</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="15" t="s">
+      <c r="A7" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="B7" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="17" t="s">
+      <c r="C7" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="0"/>
-      <c r="I7" s="0"/>
-      <c r="J7" s="0"/>
-      <c r="K7" s="0"/>
-    </row>
-    <row r="8" customFormat="false" ht="30.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="18" t="s">
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="D8" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="E8" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="3" t="n">
+      <c r="F8" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="I8" s="20" t="n">
+      <c r="I8" s="4" t="n">
         <v>10000</v>
       </c>
-      <c r="J8" s="20" t="n">
+      <c r="J8" s="4" t="n">
         <v>30000</v>
       </c>
-      <c r="K8" s="21" t="n">
+      <c r="K8" s="5" t="n">
         <v>100000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
F 780 release (#57)
</commit_message>
<xml_diff>
--- a/templates/ecommerce/template.xlsx
+++ b/templates/ecommerce/template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <r>
       <rPr>
@@ -30,9 +30,9 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="204"/>
+        <charset val="1"/>
       </rPr>
-      <t>ПРАЙС-ЛИСТ </t>
+      <t xml:space="preserve">ПРАЙС-ЛИСТ </t>
     </r>
     <r>
       <rPr>
@@ -41,9 +41,9 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="204"/>
+        <charset val="1"/>
       </rPr>
-      <t> 
+      <t xml:space="preserve"> 
 ООО "Исток-Плюс" 
 (812) 416-32-00</t>
     </r>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t xml:space="preserve">Цены указаны на:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.08.2016</t>
   </si>
   <si>
     <t xml:space="preserve">Итого товара:</t>
@@ -103,7 +106,7 @@
     <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
     <numFmt numFmtId="166" formatCode="#,##0.00&quot; р.&quot;"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -132,7 +135,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -140,7 +143,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="16"/>
@@ -150,7 +160,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -159,12 +169,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDBEEF4"/>
+        <fgColor rgb="FFBABABA"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDAEEF3"/>
         <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -173,84 +189,14 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
+      <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="medium"/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -274,108 +220,88 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="6" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="2" borderId="7" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="8" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in 20% - Accent5" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -393,12 +319,12 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFBABABA"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFDBEEF4"/>
+      <rgbColor rgb="FFDAEEF3"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
@@ -448,177 +374,203 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.3481781376518"/>
     <col collapsed="false" hidden="true" max="2" min="2" style="0" width="0"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.2105263157895"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="10" min="8" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.497975708502"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="10" min="8" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="0"/>
-      <c r="I1" s="0"/>
-      <c r="J1" s="0"/>
-      <c r="K1" s="0"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="0"/>
-      <c r="I2" s="0"/>
-      <c r="J2" s="0"/>
-      <c r="K2" s="0"/>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="0"/>
-      <c r="I3" s="0"/>
-      <c r="J3" s="0"/>
-      <c r="K3" s="0"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="3" t="s">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="21.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+    <row r="5" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="6" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="7" t="n">
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="8" t="n">
         <f aca="false">SUM(G9:G100000)</f>
         <v>0</v>
       </c>
-      <c r="H5" s="0"/>
-      <c r="I5" s="0"/>
-      <c r="J5" s="0"/>
-      <c r="K5" s="0"/>
-    </row>
-    <row r="6" s="14" customFormat="true" ht="21.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H5" s="2" t="n">
+        <f aca="false">SUM(H9:H3448)</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <f aca="false">SUM(I9:I3448)</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <f aca="false">SUM(J9:J3448)</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="3" t="n">
+        <f aca="false">SUM(K9:K3448)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" s="15" customFormat="true" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="10" t="n">
-        <f aca="false">SUM(H9:I35)</f>
+        <f aca="false">MIN(H6:K6)</f>
         <v>0</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G6" s="12" t="str">
         <f aca="false">IF(E6&gt;K8,F8,IF(E6&gt;J8,E8,IF(E6&gt;I8,D8,C8)))</f>
         <v>розница</v>
       </c>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
+      <c r="H6" s="13" t="str">
+        <f aca="false">IF(H5&gt;H8,H5,J4)</f>
+        <v>NaN</v>
+      </c>
+      <c r="I6" s="13" t="str">
+        <f aca="false">IF(I5&gt;I8,I5,J4)</f>
+        <v>NaN</v>
+      </c>
+      <c r="J6" s="13" t="str">
+        <f aca="false">IF(J5&gt;J8,J5,J4)</f>
+        <v>NaN</v>
+      </c>
+      <c r="K6" s="14" t="str">
+        <f aca="false">IF(K5&gt;K8,K5,J4)</f>
+        <v>NaN</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="15" t="s">
+      <c r="A7" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="B7" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="17" t="s">
+      <c r="C7" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="0"/>
-      <c r="I7" s="0"/>
-      <c r="J7" s="0"/>
-      <c r="K7" s="0"/>
-    </row>
-    <row r="8" customFormat="false" ht="30.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="18" t="s">
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="D8" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="E8" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="3" t="n">
+      <c r="F8" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="I8" s="20" t="n">
+      <c r="I8" s="4" t="n">
         <v>10000</v>
       </c>
-      <c r="J8" s="20" t="n">
+      <c r="J8" s="4" t="n">
         <v>30000</v>
       </c>
-      <c r="K8" s="21" t="n">
+      <c r="K8" s="5" t="n">
         <v>100000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix business changes: (#75)
* Fix business changes:

- Change header cart animation config
- Fix ftp connection for import catalog
- Autolaunch collectstatic on catalog command
- Fix price excel markup

* Fix business changes:

- Change header cart animation config
- Fix ftp connection for import catalog
- Autolaunch collectstatic on catalog command
- Fix price excel markup
</commit_message>
<xml_diff>
--- a/templates/ecommerce/template.xlsx
+++ b/templates/ecommerce/template.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Прайслист" sheetId="1" r:id="rId1"/>
     <sheet name="Лист3" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -40,9 +40,6 @@
     <t>Сумма заказа:</t>
   </si>
   <si>
-    <t>Ценовая группа:</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Наименование,Характеристика номенклатуры</t>
   </si>
   <si>
@@ -73,6 +70,9 @@
     <t>info@shopelectro.ru
 ООО "Исток-Плюс" 
 (812) 416-32-00</t>
+  </si>
+  <si>
+    <t>Тип цен:</t>
   </si>
 </sst>
 </file>
@@ -162,24 +162,6 @@
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -207,6 +189,24 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -580,202 +580,202 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.28515625"/>
+    <col min="1" max="1" width="68.140625" customWidth="1"/>
     <col min="2" max="2" width="0" hidden="1"/>
-    <col min="3" max="3" width="11.140625"/>
-    <col min="4" max="4" width="13"/>
-    <col min="5" max="5" width="18.42578125"/>
-    <col min="6" max="6" width="23.7109375"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
     <col min="7" max="7" width="22.7109375"/>
     <col min="11" max="11" width="10.42578125"/>
     <col min="12" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="2"/>
+    </row>
+    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="6">
+        <f>SUM(G9:G100000)</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <f>SUM(H9:H3448)</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <f>SUM(I9:I3448)</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <f>SUM(J9:J3448)</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <f>SUM(K9:K3448)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A6" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="16"/>
+      <c r="C6" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="17"/>
+      <c r="E6" s="7">
+        <f>MIN(H6:K6)</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="8"/>
-    </row>
-    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="8"/>
-    </row>
-    <row r="3" spans="1:11" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="8"/>
-    </row>
-    <row r="4" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="12">
-        <f>SUM(G9:G100000)</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="7">
-        <f>SUM(H9:H3448)</f>
-        <v>0</v>
-      </c>
-      <c r="I5" s="7">
-        <f>SUM(I9:I3448)</f>
-        <v>0</v>
-      </c>
-      <c r="J5" s="7">
-        <f>SUM(J9:J3448)</f>
-        <v>0</v>
-      </c>
-      <c r="K5" s="8">
-        <f>SUM(K9:K3448)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="13">
-        <f>MIN(H6:K6)</f>
-        <v>0</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="15" t="str">
+      <c r="G6" s="9" t="str">
         <f>IF(E6&gt;K8,F8,IF(E6&gt;J8,E8,IF(E6&gt;I8,D8,C8)))</f>
         <v>розница</v>
       </c>
-      <c r="H6" s="16" t="str">
+      <c r="H6" s="10" t="str">
         <f>IF(H5&gt;H8,H5,J4)</f>
         <v>NaN</v>
       </c>
-      <c r="I6" s="16" t="str">
+      <c r="I6" s="10" t="str">
         <f>IF(I5&gt;I8,I5,J4)</f>
         <v>NaN</v>
       </c>
-      <c r="J6" s="16" t="str">
+      <c r="J6" s="10" t="str">
         <f>IF(J5&gt;J8,J5,J4)</f>
         <v>NaN</v>
       </c>
-      <c r="K6" s="17" t="str">
+      <c r="K6" s="11" t="str">
         <f>IF(K5&gt;K8,K5,J4)</f>
         <v>NaN</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="8"/>
-    </row>
-    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="9" t="s">
+      <c r="D8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="E8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="F8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="9">
+      <c r="G8" s="20"/>
+      <c r="H8" s="3">
         <v>1</v>
       </c>
-      <c r="I8" s="9">
+      <c r="I8" s="3">
         <v>10000</v>
       </c>
-      <c r="J8" s="9">
+      <c r="J8" s="3">
         <v>30000</v>
       </c>
-      <c r="K8" s="10">
+      <c r="K8" s="4">
         <v>100000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[FF] Price excel column size
</commit_message>
<xml_diff>
--- a/templates/ecommerce/template.xlsx
+++ b/templates/ecommerce/template.xlsx
@@ -580,12 +580,12 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="68.140625" customWidth="1"/>
+    <col min="1" max="1" width="77.42578125" customWidth="1"/>
     <col min="2" max="2" width="0" hidden="1"/>
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" customWidth="1"/>

</xml_diff>

<commit_message>
Change wholesale bounds in price excel
</commit_message>
<xml_diff>
--- a/templates/ecommerce/template.xlsx
+++ b/templates/ecommerce/template.xlsx
@@ -55,14 +55,6 @@
     <t>розница</t>
   </si>
   <si>
-    <t>мелкий опт
-(от 15 000)</t>
-  </si>
-  <si>
-    <t>средний опт
-(от 40 000)</t>
-  </si>
-  <si>
     <t>крупный опт
 (от 100 000)</t>
   </si>
@@ -73,6 +65,14 @@
   </si>
   <si>
     <t>Тип цен:</t>
+  </si>
+  <si>
+    <t>мелкий опт
+(от 20 000)</t>
+  </si>
+  <si>
+    <t>средний опт
+(от 50 000)</t>
   </si>
 </sst>
 </file>
@@ -580,7 +580,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,7 +598,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -706,7 +706,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G6" s="9" t="str">
         <f>IF(E6&gt;K8,F8,IF(E6&gt;J8,E8,IF(E6&gt;I8,D8,C8)))</f>
@@ -757,23 +757,23 @@
         <v>10</v>
       </c>
       <c r="D8" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="13" t="s">
         <v>11</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>13</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="3">
         <v>1</v>
       </c>
       <c r="I8" s="3">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="J8" s="3">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="K8" s="4">
         <v>100000</v>

</xml_diff>

<commit_message>
Trello fixes 2311 (#93)
* Prevent 301 redirect from common area

* Fill ProductPage with metadata

* Add image microdata

* Add huckster service

* Add product_type tag for google merchant

* Change wholesale bounds in price excel

* Generate titles, change buttons for seo guys

* Fix import catalog tests

* Fix back call dependencies

* Increase prods count on category page

* Refactor loaded products count

* Refactor loaded products count

* Seo shit text suffix

* Add seo shit text pattern to categories

* Add se78 yml file for parsing

* Review fixes
</commit_message>
<xml_diff>
--- a/templates/ecommerce/template.xlsx
+++ b/templates/ecommerce/template.xlsx
@@ -55,14 +55,6 @@
     <t>розница</t>
   </si>
   <si>
-    <t>мелкий опт
-(от 15 000)</t>
-  </si>
-  <si>
-    <t>средний опт
-(от 40 000)</t>
-  </si>
-  <si>
     <t>крупный опт
 (от 100 000)</t>
   </si>
@@ -73,6 +65,14 @@
   </si>
   <si>
     <t>Тип цен:</t>
+  </si>
+  <si>
+    <t>мелкий опт
+(от 20 000)</t>
+  </si>
+  <si>
+    <t>средний опт
+(от 50 000)</t>
   </si>
 </sst>
 </file>
@@ -580,7 +580,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,7 +598,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -706,7 +706,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G6" s="9" t="str">
         <f>IF(E6&gt;K8,F8,IF(E6&gt;J8,E8,IF(E6&gt;I8,D8,C8)))</f>
@@ -757,23 +757,23 @@
         <v>10</v>
       </c>
       <c r="D8" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="13" t="s">
         <v>11</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>13</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="3">
         <v>1</v>
       </c>
       <c r="I8" s="3">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="J8" s="3">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="K8" s="4">
         <v>100000</v>

</xml_diff>